<commit_message>
adding fisher result to verification
</commit_message>
<xml_diff>
--- a/data/verification/geneset_charaterization_runtime_memory.xlsx
+++ b/data/verification/geneset_charaterization_runtime_memory.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lanier4/PycharmProjects/GeneSet_Characterization_Pipeline/data/verification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingge2/PycharmProjects/KnowEng/dev/GeneSet_Characterization_Pipeline/data/verification/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9020" yWindow="460" windowWidth="24040" windowHeight="28220" tabRatio="500"/>
+    <workbookView xWindow="1480" yWindow="460" windowWidth="24040" windowHeight="19660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DRaWR" sheetId="1" r:id="rId1"/>
+    <sheet name="fisher" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
   <si>
     <t>samples</t>
   </si>
@@ -186,6 +187,165 @@
   </si>
   <si>
     <t>function call memory total</t>
+  </si>
+  <si>
+    <t>Input Variables</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>pandas df string</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean </t>
+  </si>
+  <si>
+    <t>python integer base size</t>
+  </si>
+  <si>
+    <t>python  float base size</t>
+  </si>
+  <si>
+    <t>python empty list base size</t>
+  </si>
+  <si>
+    <t>python dict base size</t>
+  </si>
+  <si>
+    <t>spreadsheet  genes</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>spreadsheet properties</t>
+  </si>
+  <si>
+    <t>property gene edges row count</t>
+  </si>
+  <si>
+    <t>property gene edges columns</t>
+  </si>
+  <si>
+    <t>unique property name in pg_network</t>
+  </si>
+  <si>
+    <t>unique gene name in pg_network</t>
+  </si>
+  <si>
+    <t>common_gene_name between pg_network and spreadsheet</t>
+  </si>
+  <si>
+    <t>intersection on gene_name between  spreadsheet and common_gene_name</t>
+  </si>
+  <si>
+    <t>number of parallel processes</t>
+  </si>
+  <si>
+    <t>get_network_mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Line number</t>
+  </si>
+  <si>
+    <t>Size/MB</t>
+  </si>
+  <si>
+    <t>prop_gene_network_df</t>
+  </si>
+  <si>
+    <t>spreadsheet_gene_names</t>
+  </si>
+  <si>
+    <t>prop_gene_network_n1_names</t>
+  </si>
+  <si>
+    <t>prop_gene_network_n2_names</t>
+  </si>
+  <si>
+    <t>common_gene_names</t>
+  </si>
+  <si>
+    <t>common_gene_names_dict</t>
+  </si>
+  <si>
+    <t>prop_gene_network_n1_names_dict</t>
+  </si>
+  <si>
+    <t>reverse_prop_dict</t>
+  </si>
+  <si>
+    <t>universe_count</t>
+  </si>
+  <si>
+    <t>prop_gene_network_sparse</t>
+  </si>
+  <si>
+    <t>fisher_final_result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total sum </t>
+  </si>
+  <si>
+    <t>get_fisher_exact_test</t>
+  </si>
+  <si>
+    <t>overlap_count</t>
+  </si>
+  <si>
+    <t>user_count</t>
+  </si>
+  <si>
+    <t>gene_count</t>
+  </si>
+  <si>
+    <t>set_list</t>
+  </si>
+  <si>
+    <t>dimension</t>
+  </si>
+  <si>
+    <t>combinations</t>
+  </si>
+  <si>
+    <t>parallelism</t>
+  </si>
+  <si>
+    <t>Total sum</t>
+  </si>
+  <si>
+    <t>fisher_exact_worker</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>pvalue</t>
+  </si>
+  <si>
+    <t>row_item</t>
+  </si>
+  <si>
+    <t>save_fisher_test_result</t>
+  </si>
+  <si>
+    <t>df_col</t>
+  </si>
+  <si>
+    <t>result_df</t>
+  </si>
+  <si>
+    <t>new_result_df</t>
   </si>
 </sst>
 </file>
@@ -268,7 +428,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -310,6 +470,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -593,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1617,4 +1778,745 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>288</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>9035</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14">
+        <v>139</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>25448</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>303</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>6959</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19">
+        <v>4239</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20">
+        <v>16751</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="8">
+        <f>C43+C55+B21*C64</f>
+        <v>30.277636000000001</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f>B13*B14*B5/B2</f>
+        <v>10.04692</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <f>B15*B16*B5/B2</f>
+        <v>0.61075199999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>30</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <f>(B11+B13*B4)/B2</f>
+        <v>7.2344000000000006E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>32</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30">
+        <f>(B11+B17*B4)/B2</f>
+        <v>2.4880000000000002E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>33</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31">
+        <f>(B11+ B18*B4)/B2</f>
+        <v>5.5736000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32">
+        <f>(B11+ B19*B4)/B2</f>
+        <v>3.3975999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33">
+        <f>196704/B2</f>
+        <v>0.19670399999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34">
+        <f>12384/B2</f>
+        <v>1.2383999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35">
+        <f>12384/B2</f>
+        <v>1.2383999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <f>B19*B14*B6/B2</f>
+        <v>4.713768</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37">
+        <f>B20*B16*B6/B2</f>
+        <v>0.40202399999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38">
+        <f>C37</f>
+        <v>0.40202399999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <f>C37</f>
+        <v>0.40202399999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40">
+        <f>B9/B2</f>
+        <v>2.8E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41">
+        <f>B19*B17*B6/B2</f>
+        <v>10.275335999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42">
+        <f>C73</f>
+        <v>2.3597839999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43">
+        <f>SUM(C27:C42)</f>
+        <v>29.598676000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>317</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47">
+        <f>B9/B2</f>
+        <v>2.8E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>318</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48">
+        <f>B17*B14*B5/B2</f>
+        <v>0.33693600000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>319</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49">
+        <f>B14*B5/B2</f>
+        <v>1.1119999999999999E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>320</v>
+      </c>
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50">
+        <f>B17*B5/B2</f>
+        <v>2.4239999999999999E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>321</v>
+      </c>
+      <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51">
+        <f>(B11+B14*B5)/B2</f>
+        <v>1.176E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>323</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52">
+        <f>(B11+2*B5)/B2</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>324</v>
+      </c>
+      <c r="B53" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53">
+        <f>(B11+B17*B14*B5)/B2</f>
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>325</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54">
+        <f>B9/B2</f>
+        <v>2.8E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55">
+        <f>SUM(C47:C54)</f>
+        <v>0.67878400000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>373</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61">
+        <f>4*B5/B2</f>
+        <v>3.1999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>374</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <f>B10/B2</f>
+        <v>2.4000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>375</v>
+      </c>
+      <c r="B63" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63">
+        <f>(B11+7*B6)/B2</f>
+        <v>1.2E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64">
+        <f>SUM(C61:C63)</f>
+        <v>1.76E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>389</v>
+      </c>
+      <c r="B70" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70">
+        <f>(B11+7*B4)/B2</f>
+        <v>1.2E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>392</v>
+      </c>
+      <c r="B71" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71">
+        <f>B14*B17*7*B6/B2</f>
+        <v>2.358552</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>396</v>
+      </c>
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72">
+        <f>B14*B3/B2</f>
+        <v>1.1119999999999999E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73">
+        <f>SUM(C70:C72)</f>
+        <v>2.3597839999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated line numbers, variables
</commit_message>
<xml_diff>
--- a/data/verification/geneset_charaterization_runtime_memory.xlsx
+++ b/data/verification/geneset_charaterization_runtime_memory.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingge2/PycharmProjects/KnowEng/dev/GeneSet_Characterization_Pipeline/data/verification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lanier4/zz_lcl_KnowEnG/GeneSet_Characterization_Pipeline/data/verification/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="460" windowWidth="24040" windowHeight="19660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="26880" yWindow="460" windowWidth="23000" windowHeight="28180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DRaWR" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>samples</t>
   </si>
@@ -345,7 +345,10 @@
     <t>result_df</t>
   </si>
   <si>
-    <t>new_result_df</t>
+    <t>result_df_with_score</t>
+  </si>
+  <si>
+    <t>result_df_with_rank</t>
   </si>
 </sst>
 </file>
@@ -754,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1664,7 +1667,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>30</v>
@@ -1782,15 +1785,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
   </cols>
@@ -2033,20 +2036,20 @@
       </c>
       <c r="B22" s="8">
         <f>C43+C55+B21*C64</f>
-        <v>30.277636000000001</v>
+        <v>30.278748</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2057,7 +2060,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+      <c r="A27" s="1">
         <v>27</v>
       </c>
       <c r="B27" t="s">
@@ -2069,7 +2072,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+      <c r="A28" s="1">
         <v>28</v>
       </c>
       <c r="B28" t="s">
@@ -2081,7 +2084,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+      <c r="A29" s="1">
         <v>30</v>
       </c>
       <c r="B29" s="17" t="s">
@@ -2093,7 +2096,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
+      <c r="A30" s="1">
         <v>32</v>
       </c>
       <c r="B30" s="17" t="s">
@@ -2105,7 +2108,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
+      <c r="A31" s="1">
         <v>33</v>
       </c>
       <c r="B31" s="17" t="s">
@@ -2117,7 +2120,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+      <c r="A32" s="1">
         <v>37</v>
       </c>
       <c r="B32" t="s">
@@ -2129,7 +2132,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
+      <c r="A33" s="1">
         <v>38</v>
       </c>
       <c r="B33" t="s">
@@ -2141,7 +2144,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
+      <c r="A34" s="1">
         <v>39</v>
       </c>
       <c r="B34" t="s">
@@ -2153,7 +2156,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
+      <c r="A35" s="1">
         <v>40</v>
       </c>
       <c r="B35" t="s">
@@ -2165,7 +2168,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+      <c r="A36" s="1">
         <v>44</v>
       </c>
       <c r="B36" t="s">
@@ -2177,7 +2180,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
+      <c r="A37" s="1">
         <v>45</v>
       </c>
       <c r="B37" t="s">
@@ -2189,8 +2192,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
-        <v>49</v>
+      <c r="A38" s="1">
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>77</v>
@@ -2201,8 +2204,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
-        <v>51</v>
+      <c r="A39" s="1">
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
@@ -2213,8 +2216,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
-        <v>56</v>
+      <c r="A40" s="1">
+        <v>57</v>
       </c>
       <c r="B40" t="s">
         <v>85</v>
@@ -2225,8 +2228,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>57</v>
+      <c r="A41" s="1">
+        <v>58</v>
       </c>
       <c r="B41" t="s">
         <v>86</v>
@@ -2237,15 +2240,15 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
-        <v>61</v>
+      <c r="A42" s="1">
+        <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>87</v>
       </c>
       <c r="C42">
-        <f>C73</f>
-        <v>2.3597839999999999</v>
+        <f>C74</f>
+        <v>2.3608959999999999</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2254,17 +2257,17 @@
       </c>
       <c r="C43">
         <f>SUM(C27:C42)</f>
-        <v>29.598676000000001</v>
+        <v>29.599788</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -2275,7 +2278,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
+      <c r="A47" s="1">
         <v>317</v>
       </c>
       <c r="B47" t="s">
@@ -2287,7 +2290,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
+      <c r="A48" s="1">
         <v>318</v>
       </c>
       <c r="B48" t="s">
@@ -2299,7 +2302,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
+      <c r="A49" s="1">
         <v>319</v>
       </c>
       <c r="B49" t="s">
@@ -2311,7 +2314,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+      <c r="A50" s="1">
         <v>320</v>
       </c>
       <c r="B50" t="s">
@@ -2323,7 +2326,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
+      <c r="A51" s="1">
         <v>321</v>
       </c>
       <c r="B51" t="s">
@@ -2335,7 +2338,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
+      <c r="A52" s="1">
         <v>323</v>
       </c>
       <c r="B52" t="s">
@@ -2347,7 +2350,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
+      <c r="A53" s="1">
         <v>324</v>
       </c>
       <c r="B53" t="s">
@@ -2359,7 +2362,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
+      <c r="A54" s="1">
         <v>325</v>
       </c>
       <c r="B54" t="s">
@@ -2371,7 +2374,6 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
       <c r="B55" t="s">
         <v>97</v>
       </c>
@@ -2380,23 +2382,14 @@
         <v>0.67878400000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="6"/>
-    </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C59" s="6"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -2407,8 +2400,8 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="6">
-        <v>373</v>
+      <c r="A61" s="1">
+        <v>374</v>
       </c>
       <c r="B61" t="s">
         <v>99</v>
@@ -2419,8 +2412,8 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="6">
-        <v>374</v>
+      <c r="A62" s="1">
+        <v>379</v>
       </c>
       <c r="B62" t="s">
         <v>100</v>
@@ -2431,8 +2424,8 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="6">
-        <v>375</v>
+      <c r="A63" s="1">
+        <v>377</v>
       </c>
       <c r="B63" t="s">
         <v>101</v>
@@ -2451,17 +2444,14 @@
         <v>1.76E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="6"/>
-    </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C68" s="6"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -2472,8 +2462,8 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="6">
-        <v>389</v>
+      <c r="A70" s="1">
+        <v>392</v>
       </c>
       <c r="B70" t="s">
         <v>103</v>
@@ -2484,8 +2474,8 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="6">
-        <v>392</v>
+      <c r="A71" s="1">
+        <v>394</v>
       </c>
       <c r="B71" t="s">
         <v>104</v>
@@ -2496,8 +2486,8 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="6">
-        <v>396</v>
+      <c r="A72" s="1">
+        <v>397</v>
       </c>
       <c r="B72" t="s">
         <v>105</v>
@@ -2508,12 +2498,24 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>402</v>
+      </c>
       <c r="B73" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73">
+        <f>B14*B3/B2</f>
+        <v>1.1119999999999999E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
         <v>97</v>
       </c>
-      <c r="C73">
-        <f>SUM(C70:C72)</f>
-        <v>2.3597839999999999</v>
+      <c r="C74">
+        <f>SUM(C70:C73)</f>
+        <v>2.3608959999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>